<commit_message>
Projektplan für PUngewiß aktualisiert.
</commit_message>
<xml_diff>
--- a/Projektplan.xlsx
+++ b/Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testdisk-7.2-WIP.win64\testdisk-7.2-WIP\backup\old_notebook\old_notebook\Desktop\RestoreFirstInstallationT580\anderScore\GitLab-Training\gitlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD78E82-42EE-4294-B455-2E8C738BDFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F44EB-3733-4E13-B885-4FDA940C2206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1249,22 +1249,19 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1277,14 +1274,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1865,8 +1865,8 @@
   </sheetPr>
   <dimension ref="A1:BN39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="V13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BP32" sqref="BP32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1892,28 +1892,28 @@
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="126">
+      <c r="Q1" s="125">
         <v>43956</v>
       </c>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
     </row>
     <row r="2" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="87" t="s">
@@ -1923,28 +1923,28 @@
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="I2" s="128" t="s">
+      <c r="I2" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="124">
+      <c r="Q2" s="123">
         <v>1</v>
       </c>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="124"/>
+      <c r="X2" s="124"/>
+      <c r="Y2" s="124"/>
+      <c r="Z2" s="124"/>
     </row>
     <row r="3" spans="1:65" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1956,102 +1956,102 @@
       <c r="A4" s="8"/>
       <c r="B4" s="23"/>
       <c r="E4" s="24"/>
-      <c r="I4" s="132">
+      <c r="I4" s="120">
         <f>I5</f>
         <v>43956</v>
       </c>
-      <c r="J4" s="130"/>
-      <c r="K4" s="130"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="130"/>
-      <c r="O4" s="130"/>
-      <c r="P4" s="130">
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="118"/>
+      <c r="P4" s="118">
         <f>P5</f>
         <v>43963</v>
       </c>
-      <c r="Q4" s="130"/>
-      <c r="R4" s="130"/>
-      <c r="S4" s="130"/>
-      <c r="T4" s="130"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="130"/>
-      <c r="W4" s="130">
+      <c r="Q4" s="118"/>
+      <c r="R4" s="118"/>
+      <c r="S4" s="118"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="118">
         <f>W5</f>
         <v>43970</v>
       </c>
-      <c r="X4" s="130"/>
-      <c r="Y4" s="130"/>
-      <c r="Z4" s="130"/>
-      <c r="AA4" s="130"/>
-      <c r="AB4" s="130"/>
-      <c r="AC4" s="130"/>
-      <c r="AD4" s="130">
+      <c r="X4" s="118"/>
+      <c r="Y4" s="118"/>
+      <c r="Z4" s="118"/>
+      <c r="AA4" s="118"/>
+      <c r="AB4" s="118"/>
+      <c r="AC4" s="118"/>
+      <c r="AD4" s="118">
         <f>AD5</f>
         <v>43977</v>
       </c>
-      <c r="AE4" s="130"/>
-      <c r="AF4" s="130"/>
-      <c r="AG4" s="130"/>
-      <c r="AH4" s="130"/>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="130"/>
-      <c r="AK4" s="130">
+      <c r="AE4" s="118"/>
+      <c r="AF4" s="118"/>
+      <c r="AG4" s="118"/>
+      <c r="AH4" s="118"/>
+      <c r="AI4" s="118"/>
+      <c r="AJ4" s="118"/>
+      <c r="AK4" s="118">
         <f>AK5</f>
         <v>43984</v>
       </c>
-      <c r="AL4" s="130"/>
-      <c r="AM4" s="130"/>
-      <c r="AN4" s="130"/>
-      <c r="AO4" s="130"/>
-      <c r="AP4" s="130"/>
-      <c r="AQ4" s="130"/>
-      <c r="AR4" s="130">
+      <c r="AL4" s="118"/>
+      <c r="AM4" s="118"/>
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118">
         <f>AR5</f>
         <v>43991</v>
       </c>
-      <c r="AS4" s="130"/>
-      <c r="AT4" s="130"/>
-      <c r="AU4" s="130"/>
-      <c r="AV4" s="130"/>
-      <c r="AW4" s="130"/>
-      <c r="AX4" s="130"/>
-      <c r="AY4" s="130">
+      <c r="AS4" s="118"/>
+      <c r="AT4" s="118"/>
+      <c r="AU4" s="118"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118">
         <f>AY5</f>
         <v>43998</v>
       </c>
-      <c r="AZ4" s="130"/>
-      <c r="BA4" s="130"/>
-      <c r="BB4" s="130"/>
-      <c r="BC4" s="130"/>
-      <c r="BD4" s="130"/>
-      <c r="BE4" s="130"/>
-      <c r="BF4" s="130">
+      <c r="AZ4" s="118"/>
+      <c r="BA4" s="118"/>
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
+      <c r="BF4" s="118">
         <f>BF5</f>
         <v>44005</v>
       </c>
-      <c r="BG4" s="130"/>
-      <c r="BH4" s="130"/>
-      <c r="BI4" s="130"/>
-      <c r="BJ4" s="130"/>
-      <c r="BK4" s="130"/>
-      <c r="BL4" s="131"/>
+      <c r="BG4" s="118"/>
+      <c r="BH4" s="118"/>
+      <c r="BI4" s="118"/>
+      <c r="BJ4" s="118"/>
+      <c r="BK4" s="118"/>
+      <c r="BL4" s="119"/>
     </row>
     <row r="5" spans="1:65" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="118"/>
-      <c r="B5" s="119" t="s">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="123" t="s">
+      <c r="D5" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="123" t="s">
+      <c r="F5" s="121" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="25">
@@ -2280,8 +2280,8 @@
       </c>
     </row>
     <row r="6" spans="1:65" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118"/>
-      <c r="B6" s="120"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="122"/>
       <c r="D6" s="122"/>
       <c r="E6" s="122"/>
@@ -2689,10 +2689,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="88">
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="F9" s="88">
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="5">
@@ -3467,7 +3467,7 @@
         <v>42</v>
       </c>
       <c r="D19" s="56">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E19" s="90">
         <v>43972</v>
@@ -3705,15 +3705,15 @@
         <v>0</v>
       </c>
       <c r="E22" s="91">
-        <v>43974</v>
+        <v>43978</v>
       </c>
       <c r="F22" s="91">
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
@@ -3784,15 +3784,15 @@
         <v>0</v>
       </c>
       <c r="E23" s="91">
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="F23" s="91">
-        <v>43977</v>
+        <v>43979</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
@@ -4909,6 +4909,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4917,16 +4927,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D36">
     <cfRule type="dataBar" priority="23">
@@ -5040,12 +5040,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5361,29 +5372,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5410,20 +5421,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tag-3_2: Neues Projekt sowie neue Pipeline erstellen.
</commit_message>
<xml_diff>
--- a/Projektplan.xlsx
+++ b/Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testdisk-7.2-WIP.win64\testdisk-7.2-WIP\backup\old_notebook\old_notebook\Desktop\RestoreFirstInstallationT580\anderScore\GitLab-Training\gitlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261F85BD-5863-449D-B01F-48DD9F1359D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1671FE3-E9D9-4552-BCF1-D872C85DBDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1249,19 +1249,22 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1274,17 +1277,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1866,7 +1866,7 @@
   <dimension ref="A1:BN39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1892,28 +1892,28 @@
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="127" t="s">
+      <c r="I1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="125">
+      <c r="Q1" s="126">
         <v>43956</v>
       </c>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
     </row>
     <row r="2" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="87" t="s">
@@ -1923,28 +1923,28 @@
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="I2" s="127" t="s">
+      <c r="I2" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="123">
+      <c r="Q2" s="124">
         <v>1</v>
       </c>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
-      <c r="Y2" s="124"/>
-      <c r="Z2" s="124"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
     </row>
     <row r="3" spans="1:65" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1956,102 +1956,102 @@
       <c r="A4" s="8"/>
       <c r="B4" s="23"/>
       <c r="E4" s="24"/>
-      <c r="I4" s="120">
+      <c r="I4" s="132">
         <f>I5</f>
         <v>43956</v>
       </c>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118">
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="130"/>
+      <c r="P4" s="130">
         <f>P5</f>
         <v>43963</v>
       </c>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118">
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
+      <c r="W4" s="130">
         <f>W5</f>
         <v>43970</v>
       </c>
-      <c r="X4" s="118"/>
-      <c r="Y4" s="118"/>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118">
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="130"/>
+      <c r="AC4" s="130"/>
+      <c r="AD4" s="130">
         <f>AD5</f>
         <v>43977</v>
       </c>
-      <c r="AE4" s="118"/>
-      <c r="AF4" s="118"/>
-      <c r="AG4" s="118"/>
-      <c r="AH4" s="118"/>
-      <c r="AI4" s="118"/>
-      <c r="AJ4" s="118"/>
-      <c r="AK4" s="118">
+      <c r="AE4" s="130"/>
+      <c r="AF4" s="130"/>
+      <c r="AG4" s="130"/>
+      <c r="AH4" s="130"/>
+      <c r="AI4" s="130"/>
+      <c r="AJ4" s="130"/>
+      <c r="AK4" s="130">
         <f>AK5</f>
         <v>43984</v>
       </c>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118">
+      <c r="AL4" s="130"/>
+      <c r="AM4" s="130"/>
+      <c r="AN4" s="130"/>
+      <c r="AO4" s="130"/>
+      <c r="AP4" s="130"/>
+      <c r="AQ4" s="130"/>
+      <c r="AR4" s="130">
         <f>AR5</f>
         <v>43991</v>
       </c>
-      <c r="AS4" s="118"/>
-      <c r="AT4" s="118"/>
-      <c r="AU4" s="118"/>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118">
+      <c r="AS4" s="130"/>
+      <c r="AT4" s="130"/>
+      <c r="AU4" s="130"/>
+      <c r="AV4" s="130"/>
+      <c r="AW4" s="130"/>
+      <c r="AX4" s="130"/>
+      <c r="AY4" s="130">
         <f>AY5</f>
         <v>43998</v>
       </c>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
-      <c r="BF4" s="118">
+      <c r="AZ4" s="130"/>
+      <c r="BA4" s="130"/>
+      <c r="BB4" s="130"/>
+      <c r="BC4" s="130"/>
+      <c r="BD4" s="130"/>
+      <c r="BE4" s="130"/>
+      <c r="BF4" s="130">
         <f>BF5</f>
         <v>44005</v>
       </c>
-      <c r="BG4" s="118"/>
-      <c r="BH4" s="118"/>
-      <c r="BI4" s="118"/>
-      <c r="BJ4" s="118"/>
-      <c r="BK4" s="118"/>
-      <c r="BL4" s="119"/>
+      <c r="BG4" s="130"/>
+      <c r="BH4" s="130"/>
+      <c r="BI4" s="130"/>
+      <c r="BJ4" s="130"/>
+      <c r="BK4" s="130"/>
+      <c r="BL4" s="131"/>
     </row>
     <row r="5" spans="1:65" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130" t="s">
+      <c r="A5" s="118"/>
+      <c r="B5" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="121" t="s">
+      <c r="D5" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="121" t="s">
+      <c r="E5" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="121" t="s">
+      <c r="F5" s="123" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="25">
@@ -2280,8 +2280,8 @@
       </c>
     </row>
     <row r="6" spans="1:65" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
-      <c r="B6" s="131"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="120"/>
       <c r="C6" s="122"/>
       <c r="D6" s="122"/>
       <c r="E6" s="122"/>
@@ -3706,18 +3706,18 @@
         <v>42</v>
       </c>
       <c r="D22" s="65">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E22" s="91">
         <v>43977</v>
       </c>
       <c r="F22" s="91">
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
@@ -4915,16 +4915,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4933,6 +4923,16 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D36">
     <cfRule type="dataBar" priority="23">
@@ -5046,23 +5046,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5378,29 +5367,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5427,9 +5416,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>